<commit_message>
Loaded some data into the database
</commit_message>
<xml_diff>
--- a/dev/db samples.xlsx
+++ b/dev/db samples.xlsx
@@ -8,17 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fguerrero\OneDrive - Linear Chemicals,SLU\Documentos\R\db.samples\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D455AD9F-4BA4-46EE-8274-767B15B25DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA21E94-6FB0-41B2-85A7-D7E36F7E0CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{DF3FA577-6866-4ED4-B8F5-3A12890ED023}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{DF3FA577-6866-4ED4-B8F5-3A12890ED023}"/>
   </bookViews>
   <sheets>
-    <sheet name="suppliers" sheetId="5" r:id="rId1"/>
-    <sheet name="supplier_references" sheetId="4" r:id="rId2"/>
-    <sheet name="supplier_lots" sheetId="3" r:id="rId3"/>
-    <sheet name="lot_changes" sheetId="2" r:id="rId4"/>
-    <sheet name="notas viejas" sheetId="1" r:id="rId5"/>
-    <sheet name="lots" sheetId="6" r:id="rId6"/>
+    <sheet name="sample_categories" sheetId="9" r:id="rId1"/>
+    <sheet name="samples" sheetId="8" r:id="rId2"/>
+    <sheet name="sample_others" sheetId="7" r:id="rId3"/>
+    <sheet name="suppliers" sheetId="5" r:id="rId4"/>
+    <sheet name="supplier_references" sheetId="4" r:id="rId5"/>
+    <sheet name="supplier_lots" sheetId="3" r:id="rId6"/>
+    <sheet name="lot_changes" sheetId="2" r:id="rId7"/>
+    <sheet name="notas viejas" sheetId="1" r:id="rId8"/>
+    <sheet name="lots" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="161">
   <si>
     <t>sample</t>
   </si>
@@ -493,10 +496,37 @@
     <t>new_lot</t>
   </si>
   <si>
-    <t>original_supplier</t>
-  </si>
-  <si>
-    <t>new_supplier</t>
+    <t>original_id_supplier</t>
+  </si>
+  <si>
+    <t>new_id_supplier</t>
+  </si>
+  <si>
+    <t>id_sample</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>id_category</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>mixture</t>
+  </si>
+  <si>
+    <t>Saline solution (0.9%)</t>
+  </si>
+  <si>
+    <t>1980099</t>
+  </si>
+  <si>
+    <t>1985099</t>
+  </si>
+  <si>
+    <t>1975090</t>
   </si>
 </sst>
 </file>
@@ -562,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -582,9 +612,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -898,6 +925,462 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2A43F5A-AA21-4E64-9D93-DCE055560ED6}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4CF8404-C1DF-44A5-BBD9-6FF4E7B6FC6A}">
+  <dimension ref="A1:B44"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F1BB0C1-AC09-4297-A20D-BD53F513C1C4}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F096EF72-053F-4EDF-A5AF-A9015E190A19}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -968,144 +1451,116 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5673DA9F-AE8B-4177-A5A3-43BADCF308D8}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="59.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.5703125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>97</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>5</v>
+        <v>82</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>93</v>
+      <c r="B2" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>93</v>
+      <c r="B3" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>93</v>
+      <c r="B4" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>92</v>
+      <c r="B5" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
-        <v>92</v>
+      <c r="B6" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="8">
+      <c r="B7" s="8">
         <v>1975090</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
-      <c r="B8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C8" s="8">
+      <c r="B8" s="8">
         <v>1980099</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" s="8">
+      <c r="B9" s="8">
         <v>1985099</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="C9" s="8" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1114,686 +1569,812 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F14917-6581-4147-ACAA-4C324253E592}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>2</v>
-      </c>
       <c r="E1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
-        <v>2</v>
-      </c>
-      <c r="B2" s="8" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
-        <v>2</v>
-      </c>
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
-        <v>2</v>
-      </c>
-      <c r="B4" s="8" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
-        <v>2</v>
-      </c>
-      <c r="B5" s="8" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="E5" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
-        <v>2</v>
-      </c>
-      <c r="B6" s="8" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
-        <v>2</v>
-      </c>
-      <c r="B7" s="8" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="E7" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
-        <v>2</v>
-      </c>
-      <c r="B8" s="8" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="E8" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
-        <v>2</v>
-      </c>
-      <c r="B9" s="8" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="D9" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="E9" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2">
         <v>3</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="C10" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="E10" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2">
         <v>3</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="C11" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="D11" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="E11" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2">
         <v>3</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="C12" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="D12" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="E12" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
-        <v>2</v>
-      </c>
-      <c r="B13" s="8" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="D13" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="E13" s="8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
-        <v>2</v>
-      </c>
-      <c r="B14" s="8" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="D14" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
-        <v>2</v>
-      </c>
-      <c r="B15" s="8" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>16</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="D15" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="E15" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
-        <v>2</v>
-      </c>
-      <c r="B16" s="8" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>17</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="D16" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="E16" s="8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
-        <v>2</v>
-      </c>
-      <c r="B17" s="8" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>18</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="D17" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="E17" s="8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
-        <v>1</v>
-      </c>
-      <c r="B18" s="8">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>19</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="8">
         <v>1980099</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="D18" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="E18" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="F18" s="8" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
-        <v>1</v>
-      </c>
-      <c r="B19" s="8">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>20</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" s="8">
         <v>1980099</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="D19" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="E19" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="F19" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
-        <v>1</v>
-      </c>
-      <c r="B20" s="8">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>21</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="8">
         <v>1985099</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="D20" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="E20" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="F20" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
-        <v>1</v>
-      </c>
-      <c r="B21" s="8">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>22</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="8">
         <v>1975090</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="D21" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="E21" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="F21" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
-        <v>1</v>
-      </c>
-      <c r="B22" s="8">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>23</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+      <c r="C22" s="8">
         <v>1980099</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="D22" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="E22" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="F22" s="8" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
-        <v>1</v>
-      </c>
-      <c r="B23" s="8">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>24</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="8">
         <v>1985099</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="D23" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="E23" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="F23" s="8" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
-        <v>1</v>
-      </c>
-      <c r="B24" s="8">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>25</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="8">
         <v>1980099</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="D24" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="E24" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="F24" s="8" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
-        <v>1</v>
-      </c>
-      <c r="B25" s="8">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>26</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="C25" s="8">
         <v>1985099</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="D25" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="E25" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="F25" s="8" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
-        <v>1</v>
-      </c>
-      <c r="B26" s="8">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>27</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1</v>
+      </c>
+      <c r="C26" s="8">
         <v>1980099</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="D26" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="E26" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="F26" s="8" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
-        <v>1</v>
-      </c>
-      <c r="B27" s="8">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>28</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
+      <c r="C27" s="8">
         <v>1985099</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="D27" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="E27" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="F27" s="8" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
-        <v>1</v>
-      </c>
-      <c r="B28" s="8">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>29</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" s="8">
         <v>1975090</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="D28" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="E28" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="F28" s="8" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
-        <v>1</v>
-      </c>
-      <c r="B29" s="8">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>30</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
+      <c r="C29" s="8">
         <v>1980099</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="D29" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="E29" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="F29" s="8" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
-        <v>1</v>
-      </c>
-      <c r="B30" s="8">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>31</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+      <c r="C30" s="8">
         <v>1985099</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="D30" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="E30" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="F30" s="8" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
-        <v>1</v>
-      </c>
-      <c r="B31" s="8">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>32</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1</v>
+      </c>
+      <c r="C31" s="8">
         <v>1985099</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="D31" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="E31" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="F31" s="8" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="9">
-        <v>1</v>
-      </c>
-      <c r="B32" s="8">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>33</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1</v>
+      </c>
+      <c r="C32" s="8">
         <v>1975090</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="D32" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="E32" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="F32" s="8" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="9">
-        <v>1</v>
-      </c>
-      <c r="B33" s="8">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>34</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1</v>
+      </c>
+      <c r="C33" s="8">
         <v>1975090</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="D33" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="E33" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="F33" s="8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="9">
-        <v>1</v>
-      </c>
-      <c r="B34" s="8">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>35</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1</v>
+      </c>
+      <c r="C34" s="8">
         <v>1980099</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="D34" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="E34" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="F34" s="8" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="9">
-        <v>1</v>
-      </c>
-      <c r="B35" s="8">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>36</v>
+      </c>
+      <c r="B35" s="2">
+        <v>1</v>
+      </c>
+      <c r="C35" s="8">
         <v>1985099</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="D35" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="E35" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="F35" s="8" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="9">
-        <v>1</v>
-      </c>
-      <c r="B36" s="8">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>37</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1</v>
+      </c>
+      <c r="C36" s="8">
         <v>1980099</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="D36" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="E36" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="F36" s="8" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="9">
-        <v>1</v>
-      </c>
-      <c r="B37" s="8">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>38</v>
+      </c>
+      <c r="B37" s="2">
+        <v>1</v>
+      </c>
+      <c r="C37" s="8">
         <v>1980099</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="D37" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="E37" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="F37" s="8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="9">
-        <v>1</v>
-      </c>
-      <c r="B38" s="8">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>39</v>
+      </c>
+      <c r="B38" s="2">
+        <v>1</v>
+      </c>
+      <c r="C38" s="8">
         <v>1985099</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="D38" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="E38" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="F38" s="8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="9">
-        <v>1</v>
-      </c>
-      <c r="B39" s="8">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>40</v>
+      </c>
+      <c r="B39" s="2">
+        <v>1</v>
+      </c>
+      <c r="C39" s="8">
         <v>1985099</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="D39" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="E39" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="F39" s="8" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="9">
-        <v>1</v>
-      </c>
-      <c r="B40" s="8">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>41</v>
+      </c>
+      <c r="B40" s="2">
+        <v>1</v>
+      </c>
+      <c r="C40" s="8">
         <v>1975090</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="D40" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="E40" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="F40" s="8" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="9">
-        <v>1</v>
-      </c>
-      <c r="B41" s="8">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>42</v>
+      </c>
+      <c r="B41" s="2">
+        <v>1</v>
+      </c>
+      <c r="C41" s="8">
         <v>1980099</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="D41" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="E41" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="F41" s="8" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="9">
-        <v>1</v>
-      </c>
-      <c r="B42" s="8">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>43</v>
+      </c>
+      <c r="B42" s="2">
+        <v>1</v>
+      </c>
+      <c r="C42" s="8">
         <v>1985099</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="D42" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="E42" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="F42" s="8" t="s">
         <v>144</v>
       </c>
     </row>
@@ -1802,20 +2383,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{757775BE-CA6F-4779-BB65-728F0B2959E1}">
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1841,8 +2422,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>93</v>
+      <c r="A2">
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>49</v>
@@ -1850,19 +2431,19 @@
       <c r="C2" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2">
-        <v>1980099</v>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>158</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>93</v>
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>49</v>
@@ -1870,19 +2451,19 @@
       <c r="C3" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3">
-        <v>1980099</v>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>158</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>93</v>
+      <c r="A4">
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>53</v>
@@ -1890,19 +2471,19 @@
       <c r="C4" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E4">
-        <v>1985099</v>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>159</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>93</v>
+      <c r="A5">
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>56</v>
@@ -1910,19 +2491,19 @@
       <c r="C5" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E5">
-        <v>1975090</v>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>160</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>93</v>
+      <c r="A6">
+        <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>49</v>
@@ -1930,19 +2511,19 @@
       <c r="C6" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E6">
-        <v>1980099</v>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>158</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>93</v>
+      <c r="A7">
+        <v>2</v>
       </c>
       <c r="B7" t="s">
         <v>53</v>
@@ -1950,19 +2531,19 @@
       <c r="C7" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E7">
-        <v>1985099</v>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>159</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>93</v>
+      <c r="A8">
+        <v>2</v>
       </c>
       <c r="B8" t="s">
         <v>49</v>
@@ -1970,19 +2551,19 @@
       <c r="C8" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D8" t="s">
-        <v>91</v>
-      </c>
-      <c r="E8">
-        <v>1980099</v>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>158</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>93</v>
+      <c r="A9">
+        <v>2</v>
       </c>
       <c r="B9" t="s">
         <v>53</v>
@@ -1990,19 +2571,19 @@
       <c r="C9" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E9">
-        <v>1985099</v>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>159</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>93</v>
+      <c r="A10">
+        <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>49</v>
@@ -2010,19 +2591,19 @@
       <c r="C10" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E10">
-        <v>1980099</v>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>158</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>93</v>
+      <c r="A11">
+        <v>2</v>
       </c>
       <c r="B11" t="s">
         <v>53</v>
@@ -2030,19 +2611,19 @@
       <c r="C11" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D11" t="s">
-        <v>91</v>
-      </c>
-      <c r="E11">
-        <v>1985099</v>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>159</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>93</v>
+      <c r="A12">
+        <v>2</v>
       </c>
       <c r="B12" t="s">
         <v>56</v>
@@ -2050,19 +2631,19 @@
       <c r="C12" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D12" t="s">
-        <v>91</v>
-      </c>
-      <c r="E12">
-        <v>1975090</v>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>160</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>93</v>
+      <c r="A13">
+        <v>2</v>
       </c>
       <c r="B13" t="s">
         <v>49</v>
@@ -2070,19 +2651,19 @@
       <c r="C13" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D13" t="s">
-        <v>91</v>
-      </c>
-      <c r="E13">
-        <v>1980099</v>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>158</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>93</v>
+      <c r="A14">
+        <v>2</v>
       </c>
       <c r="B14" t="s">
         <v>53</v>
@@ -2090,19 +2671,19 @@
       <c r="C14" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D14" t="s">
-        <v>91</v>
-      </c>
-      <c r="E14">
-        <v>1985099</v>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>159</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>93</v>
+      <c r="A15">
+        <v>2</v>
       </c>
       <c r="B15" t="s">
         <v>53</v>
@@ -2110,19 +2691,19 @@
       <c r="C15" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E15">
-        <v>1985099</v>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>159</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>93</v>
+      <c r="A16">
+        <v>2</v>
       </c>
       <c r="B16" t="s">
         <v>56</v>
@@ -2130,19 +2711,19 @@
       <c r="C16" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D16" t="s">
-        <v>91</v>
-      </c>
-      <c r="E16">
-        <v>1975090</v>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>160</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>93</v>
+      <c r="A17">
+        <v>2</v>
       </c>
       <c r="B17" t="s">
         <v>56</v>
@@ -2150,19 +2731,19 @@
       <c r="C17" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E17">
-        <v>1975090</v>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>160</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>92</v>
+      <c r="A18">
+        <v>3</v>
       </c>
       <c r="B18" t="s">
         <v>69</v>
@@ -2170,19 +2751,19 @@
       <c r="C18" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D18" t="s">
-        <v>91</v>
-      </c>
-      <c r="E18">
-        <v>1980099</v>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>158</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>92</v>
+      <c r="A19">
+        <v>3</v>
       </c>
       <c r="B19" t="s">
         <v>72</v>
@@ -2190,19 +2771,19 @@
       <c r="C19" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E19">
-        <v>1985099</v>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>159</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>92</v>
+      <c r="A20">
+        <v>3</v>
       </c>
       <c r="B20" t="s">
         <v>69</v>
@@ -2210,19 +2791,19 @@
       <c r="C20" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D20" t="s">
-        <v>91</v>
-      </c>
-      <c r="E20">
-        <v>1980099</v>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>158</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>93</v>
+      <c r="A21">
+        <v>2</v>
       </c>
       <c r="B21" t="s">
         <v>49</v>
@@ -2230,19 +2811,19 @@
       <c r="C21" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D21" t="s">
-        <v>91</v>
-      </c>
-      <c r="E21">
-        <v>1980099</v>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>158</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>93</v>
+      <c r="A22">
+        <v>2</v>
       </c>
       <c r="B22" t="s">
         <v>53</v>
@@ -2250,19 +2831,19 @@
       <c r="C22" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D22" t="s">
-        <v>91</v>
-      </c>
-      <c r="E22">
-        <v>1985099</v>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>159</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>93</v>
+      <c r="A23">
+        <v>2</v>
       </c>
       <c r="B23" t="s">
         <v>53</v>
@@ -2270,19 +2851,19 @@
       <c r="C23" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D23" t="s">
-        <v>91</v>
-      </c>
-      <c r="E23">
-        <v>1985099</v>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>159</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>93</v>
+      <c r="A24">
+        <v>2</v>
       </c>
       <c r="B24" t="s">
         <v>56</v>
@@ -2290,19 +2871,19 @@
       <c r="C24" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D24" t="s">
-        <v>91</v>
-      </c>
-      <c r="E24">
-        <v>1975090</v>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>160</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>93</v>
+      <c r="A25">
+        <v>2</v>
       </c>
       <c r="B25" t="s">
         <v>49</v>
@@ -2310,19 +2891,19 @@
       <c r="C25" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E25">
-        <v>1980099</v>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>158</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>93</v>
+      <c r="A26">
+        <v>2</v>
       </c>
       <c r="B26" t="s">
         <v>53</v>
@@ -2330,11 +2911,11 @@
       <c r="C26" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D26" t="s">
-        <v>91</v>
-      </c>
-      <c r="E26">
-        <v>1985099</v>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>159</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>145</v>
@@ -2345,7 +2926,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFCDEAD6-B457-4473-A9CF-8F2945D21F32}">
   <dimension ref="A1:Z15"/>
   <sheetViews>
@@ -2836,7 +3417,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F897CF0-4C48-49E7-91BD-28DC4D3F75E6}">
   <dimension ref="A1:D26"/>
   <sheetViews>

</xml_diff>